<commit_message>
clean code, implement task_timer()
</commit_message>
<xml_diff>
--- a/time_example.xlsx
+++ b/time_example.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0,00"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <name val="Calibri"/>
@@ -55,10 +57,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -424,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,8 +469,8 @@
           <t>kitchen</t>
         </is>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>9</v>
+      <c r="C4" s="4" t="n">
+        <v>12.00111111111111</v>
       </c>
     </row>
     <row r="5">
@@ -477,6 +481,36 @@
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>nowe</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>list_existing_tasks</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>0.0002777777777777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement basic response for events
</commit_message>
<xml_diff>
--- a/time_example.xlsx
+++ b/time_example.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="C4" s="4" t="n">
-        <v>12.00111111111111</v>
+        <v>13.00138888888889</v>
       </c>
     </row>
     <row r="5">
@@ -511,6 +511,32 @@
       </c>
       <c r="C8" s="4" t="n">
         <v>0.0002777777777777778</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>new test task</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="1" t="inlineStr"/>
+      <c r="C10" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>second test task</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>0.02416666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add customized task and time columns names
</commit_message>
<xml_diff>
--- a/time_example.xlsx
+++ b/time_example.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,6 +539,16 @@
         <v>0.02416666666666666</v>
       </c>
     </row>
+    <row r="12">
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>another test task</t>
+        </is>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>0.003611111111111111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>